<commit_message>
final Push All hospitals have been processed 123 ok BUT with some missing people 5 blocked for javascript or other reasons 2 closed. 9 known to need further work Review of those 9 and 3 other manual entry required tomorrow
</commit_message>
<xml_diff>
--- a/tracking/Log of Missing People.xlsx
+++ b/tracking/Log of Missing People.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ExecutiveSearchYaml\tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{070E4F01-AFB9-4701-9934-87008B8D9FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF89FD12-4980-44D5-BA15-10A6358FCB44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15780" yWindow="2500" windowWidth="16690" windowHeight="17860" xr2:uid="{EFD8C19A-3C04-4967-9040-2AA86AC641A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>FAC</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>VICE PRESIDENT FINANCE &amp; CORPORATE SERVICES</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>Manual entry D</t>
+  </si>
+  <si>
+    <t>Red Lake</t>
+  </si>
+  <si>
+    <t>Angela Bishop</t>
+  </si>
+  <si>
+    <t>Interim President</t>
+  </si>
+  <si>
+    <t>h2_name and p title</t>
+  </si>
+  <si>
+    <t>Hamilton Heatl</t>
+  </si>
+  <si>
+    <t>Rochelle Reid</t>
+  </si>
+  <si>
+    <t>Stratetic lead</t>
+  </si>
+  <si>
+    <t>div_classes</t>
   </si>
 </sst>
 </file>
@@ -441,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCD8725-06E1-4360-8721-B791862EF4BF}">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A2:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,6 +513,51 @@
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>890</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>896</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>942</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>